<commit_message>
-Completed content inventory, removed full project report docx
</commit_message>
<xml_diff>
--- a/working_documents/Milestone2/2.Content Inventory.xlsx
+++ b/working_documents/Milestone2/2.Content Inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9740" yWindow="440" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="11640" yWindow="0" windowWidth="25600" windowHeight="19040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>PAGE ID</t>
   </si>
@@ -33,10 +33,97 @@
     <t>NOTES</t>
   </si>
   <si>
-    <t>Home Page</t>
-  </si>
-  <si>
-    <t>http://www.site.com.au</t>
+    <t>The Code Fair</t>
+  </si>
+  <si>
+    <t>Sponsors</t>
+  </si>
+  <si>
+    <t>Sign Up</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
+    <t>Privacy Policy</t>
+  </si>
+  <si>
+    <t>Sitemap</t>
+  </si>
+  <si>
+    <t>Link Name</t>
+  </si>
+  <si>
+    <t>CDU Code Fair 2017</t>
+  </si>
+  <si>
+    <t>Code Fair History</t>
+  </si>
+  <si>
+    <t>Previous Code Fair Reports</t>
+  </si>
+  <si>
+    <t>https://jaybeebauer.github.io/codefair/</t>
+  </si>
+  <si>
+    <t>https://jaybeebauer.github.io/codefair/#codefair</t>
+  </si>
+  <si>
+    <t>https://jaybeebauer.github.io/codefair/#signup</t>
+  </si>
+  <si>
+    <t>https://jaybeebauer.github.io/codefair/#sponsors</t>
+  </si>
+  <si>
+    <t>https://jaybeebauer.github.io/codefair/#privacypolicy</t>
+  </si>
+  <si>
+    <t>https://jaybeebauer.github.io/codefair/#sitemap</t>
+  </si>
+  <si>
+    <t>What is the code fair about?</t>
+  </si>
+  <si>
+    <t>Can I participate in the code fair?</t>
+  </si>
+  <si>
+    <t>How do I get involved?</t>
+  </si>
+  <si>
+    <t>Past results and reports</t>
+  </si>
+  <si>
+    <t>Company's and people involved</t>
+  </si>
+  <si>
+    <t>Rules</t>
+  </si>
+  <si>
+    <t>https://jaybeebauer.github.io/codefair/#rules</t>
+  </si>
+  <si>
+    <t>Images from past events</t>
+  </si>
+  <si>
+    <t>https://jaybeebauer.github.io/codefair/fairhistory/reports.html</t>
+  </si>
+  <si>
+    <t>https://jaybeebauer.github.io/codefair/fairhistory/images.html</t>
+  </si>
+  <si>
+    <t>Only go to html page if javascript disabled, open new tab/window</t>
+  </si>
+  <si>
+    <t>https://jaybeebauer.github.io/codefair/#fairhistory</t>
+  </si>
+  <si>
+    <t>Need more information?</t>
+  </si>
+  <si>
+    <t>https://jaybeebauer.github.io/codefair/#contactus</t>
+  </si>
+  <si>
+    <t>Also show event format, information on why the code fair exists</t>
   </si>
 </sst>
 </file>
@@ -44,9 +131,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -57,6 +144,30 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -76,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -84,17 +195,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -424,21 +609,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D3"/>
+  <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="43.83203125" customWidth="1"/>
-    <col min="4" max="4" width="42.5" customWidth="1"/>
+    <col min="2" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="53" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -446,25 +631,183 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
+    <row r="3" spans="1:5">
+      <c r="A3" s="6">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="6">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="10">
+        <v>4.2</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="6">
         <v>5</v>
       </c>
+      <c r="B10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="6">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="6">
+        <v>7</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="6">
+        <v>8</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
-Adjusted notes for Content Inventory
</commit_message>
<xml_diff>
--- a/working_documents/Milestone2/2.Content Inventory.xlsx
+++ b/working_documents/Milestone2/2.Content Inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="0" windowWidth="25600" windowHeight="19040" tabRatio="500"/>
+    <workbookView xWindow="10140" yWindow="0" windowWidth="25600" windowHeight="19040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>PAGE ID</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>Also show event format, information on why the code fair exists</t>
+  </si>
+  <si>
+    <t>Sign up form, need to get what information is required</t>
+  </si>
+  <si>
+    <t>Contact us form</t>
+  </si>
+  <si>
+    <t>Need to obtain a privacy policy</t>
   </si>
 </sst>
 </file>
@@ -612,7 +621,7 @@
   <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -700,7 +709,9 @@
       <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6">
@@ -773,7 +784,9 @@
       <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6">
@@ -788,7 +801,9 @@
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6">
@@ -807,7 +822,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>